<commit_message>
added sample Rt code
</commit_message>
<xml_diff>
--- a/data/covid_admit.xlsx
+++ b/data/covid_admit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DT643/Documents/Rproject/CovidModellingReprod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC2EA9-DB04-254D-9662-D8E00A70E00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59759AEB-F49F-4F40-B206-3AB85A89A473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>new_admit</t>
   </si>
   <si>
     <t>cum_admit</t>
+  </si>
+  <si>
+    <t>datac</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:C396"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -554,13 +554,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16">

</xml_diff>